<commit_message>
Some USB speed measure improvements
</commit_message>
<xml_diff>
--- a/Tests/res_in_new_2.xlsx
+++ b/Tests/res_in_new_2.xlsx
@@ -38,40 +38,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -83,18 +54,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -106,32 +78,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -153,15 +101,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -181,6 +121,66 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -191,25 +191,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -227,12 +257,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -245,7 +269,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -257,13 +281,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -275,13 +311,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -299,7 +329,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -311,37 +347,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -353,25 +359,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -389,6 +389,26 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -424,11 +444,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -448,32 +474,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -487,148 +487,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -9708,8 +9708,8 @@
   <sheetPr/>
   <dimension ref="A1:CH602"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A195" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:D200"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.54545454545455" defaultRowHeight="18"/>
@@ -9726,10 +9726,10 @@
         <v>1</v>
       </c>
       <c r="B1" s="1">
-        <v>29319.5</v>
+        <v>28839.2</v>
       </c>
       <c r="C1" s="1">
-        <v>0.34107</v>
+        <v>0.34675</v>
       </c>
       <c r="D1" s="1">
         <v>10000</v>
@@ -9752,10 +9752,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>58078.8</v>
+        <v>59352.5</v>
       </c>
       <c r="C2" s="1">
-        <v>0.34436</v>
+        <v>0.33697</v>
       </c>
       <c r="D2" s="1">
         <v>10000</v>
@@ -9778,10 +9778,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="1">
-        <v>85394.7</v>
+        <v>83542.2</v>
       </c>
       <c r="C3" s="1">
-        <v>0.35131</v>
+        <v>0.3591</v>
       </c>
       <c r="D3" s="1">
         <v>10000</v>
@@ -9804,10 +9804,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="1">
-        <v>109200</v>
+        <v>108778</v>
       </c>
       <c r="C4" s="1">
-        <v>0.3663</v>
+        <v>0.36772</v>
       </c>
       <c r="D4" s="1">
         <v>10000</v>
@@ -9830,10 +9830,10 @@
         <v>7</v>
       </c>
       <c r="B5" s="1">
-        <v>181955</v>
+        <v>182539</v>
       </c>
       <c r="C5" s="1">
-        <v>0.38471</v>
+        <v>0.38348</v>
       </c>
       <c r="D5" s="1">
         <v>10000</v>
@@ -9872,10 +9872,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="1">
-        <v>208366</v>
+        <v>208404</v>
       </c>
       <c r="C6" s="1">
-        <v>0.38394</v>
+        <v>0.38387</v>
       </c>
       <c r="D6" s="1">
         <v>10000</v>
@@ -9914,10 +9914,10 @@
         <v>15</v>
       </c>
       <c r="B7" s="1">
-        <v>219912</v>
+        <v>220913</v>
       </c>
       <c r="C7" s="1">
-        <v>0.68209</v>
+        <v>0.679</v>
       </c>
       <c r="D7" s="1">
         <v>10000</v>
@@ -9956,10 +9956,10 @@
         <v>16</v>
       </c>
       <c r="B8" s="1">
-        <v>235360</v>
+        <v>235111</v>
       </c>
       <c r="C8" s="1">
-        <v>0.67981</v>
+        <v>0.68053</v>
       </c>
       <c r="D8" s="1">
         <v>10000</v>
@@ -9998,10 +9998,10 @@
         <v>31</v>
       </c>
       <c r="B9" s="1">
-        <v>387389</v>
+        <v>387762</v>
       </c>
       <c r="C9" s="1">
-        <v>0.80023</v>
+        <v>0.79946</v>
       </c>
       <c r="D9" s="1">
         <v>10000</v>
@@ -10040,10 +10040,10 @@
         <v>32</v>
       </c>
       <c r="B10" s="1">
-        <v>400205</v>
+        <v>400471</v>
       </c>
       <c r="C10" s="1">
-        <v>0.79959</v>
+        <v>0.79906</v>
       </c>
       <c r="D10" s="1">
         <v>10000</v>
@@ -10082,10 +10082,10 @@
         <v>63</v>
       </c>
       <c r="B11" s="1">
-        <v>520549</v>
+        <v>520528</v>
       </c>
       <c r="C11" s="1">
-        <v>1.21026</v>
+        <v>1.21031</v>
       </c>
       <c r="D11" s="1">
         <v>10000</v>
@@ -10124,10 +10124,10 @@
         <v>64</v>
       </c>
       <c r="B12" s="1">
-        <v>422964</v>
+        <v>423171</v>
       </c>
       <c r="C12" s="1">
-        <v>1.51313</v>
+        <v>1.51239</v>
       </c>
       <c r="D12" s="1">
         <v>10000</v>
@@ -10166,10 +10166,10 @@
         <v>127</v>
       </c>
       <c r="B13" s="1">
-        <v>653571</v>
+        <v>650902</v>
       </c>
       <c r="C13" s="1">
-        <v>1.94317</v>
+        <v>1.95114</v>
       </c>
       <c r="D13" s="1">
         <v>10000</v>
@@ -10208,10 +10208,10 @@
         <v>128</v>
       </c>
       <c r="B14" s="1">
-        <v>571822</v>
+        <v>572484</v>
       </c>
       <c r="C14" s="1">
-        <v>2.23846</v>
+        <v>2.23587</v>
       </c>
       <c r="D14" s="1">
         <v>10000</v>
@@ -10247,10 +10247,10 @@
         <v>255</v>
       </c>
       <c r="B15" s="1">
-        <v>751773</v>
+        <v>752237</v>
       </c>
       <c r="C15" s="1">
-        <v>3.39198</v>
+        <v>3.38989</v>
       </c>
       <c r="D15" s="1">
         <v>10000</v>
@@ -10289,10 +10289,10 @@
         <v>256</v>
       </c>
       <c r="B16" s="1">
-        <v>684543</v>
+        <v>684443</v>
       </c>
       <c r="C16" s="1">
-        <v>3.73972</v>
+        <v>3.74027</v>
       </c>
       <c r="D16" s="1">
         <v>10000</v>
@@ -10331,10 +10331,10 @@
         <v>511</v>
       </c>
       <c r="B17" s="1">
-        <v>791307</v>
+        <v>792225</v>
       </c>
       <c r="C17" s="1">
-        <v>6.45767</v>
+        <v>6.45019</v>
       </c>
       <c r="D17" s="1">
         <v>10000</v>
@@ -10373,10 +10373,10 @@
         <v>512</v>
       </c>
       <c r="B18" s="1">
-        <v>788063</v>
+        <v>787548</v>
       </c>
       <c r="C18" s="1">
-        <v>6.49694</v>
+        <v>6.50119</v>
       </c>
       <c r="D18" s="1">
         <v>10000</v>
@@ -10415,10 +10415,10 @@
         <v>1023</v>
       </c>
       <c r="B19" s="1">
-        <v>810010</v>
+        <v>811116</v>
       </c>
       <c r="C19" s="1">
-        <v>12.6295</v>
+        <v>12.6123</v>
       </c>
       <c r="D19" s="1">
         <v>10000</v>
@@ -10457,10 +10457,10 @@
         <v>1024</v>
       </c>
       <c r="B20" s="1">
-        <v>814026</v>
+        <v>813963</v>
       </c>
       <c r="C20" s="1">
-        <v>12.5794</v>
+        <v>12.5804</v>
       </c>
       <c r="D20" s="1">
         <v>10000</v>
@@ -10499,10 +10499,10 @@
         <v>1</v>
       </c>
       <c r="B21" s="1">
-        <v>29385.8</v>
+        <v>29753</v>
       </c>
       <c r="C21" s="1">
-        <v>0.3403</v>
+        <v>0.3361</v>
       </c>
       <c r="D21" s="1">
         <v>10000</v>
@@ -10541,10 +10541,10 @@
         <v>2</v>
       </c>
       <c r="B22" s="1">
-        <v>57873.7</v>
+        <v>58307.3</v>
       </c>
       <c r="C22" s="1">
-        <v>0.34558</v>
+        <v>0.34301</v>
       </c>
       <c r="D22" s="1">
         <v>10000</v>
@@ -10583,10 +10583,10 @@
         <v>3</v>
       </c>
       <c r="B23" s="1">
-        <v>83222.4</v>
+        <v>83393.6</v>
       </c>
       <c r="C23" s="1">
-        <v>0.36048</v>
+        <v>0.35974</v>
       </c>
       <c r="D23" s="1">
         <v>10000</v>
@@ -10625,10 +10625,10 @@
         <v>4</v>
       </c>
       <c r="B24" s="1">
-        <v>109278</v>
+        <v>109430</v>
       </c>
       <c r="C24" s="1">
-        <v>0.36604</v>
+        <v>0.36553</v>
       </c>
       <c r="D24" s="1">
         <v>10000</v>
@@ -10667,10 +10667,10 @@
         <v>7</v>
       </c>
       <c r="B25" s="1">
-        <v>181927</v>
+        <v>182834</v>
       </c>
       <c r="C25" s="1">
-        <v>0.38477</v>
+        <v>0.38286</v>
       </c>
       <c r="D25" s="1">
         <v>10000</v>
@@ -10709,10 +10709,10 @@
         <v>8</v>
       </c>
       <c r="B26" s="1">
-        <v>208035</v>
+        <v>208328</v>
       </c>
       <c r="C26" s="1">
-        <v>0.38455</v>
+        <v>0.38401</v>
       </c>
       <c r="D26" s="1">
         <v>10000</v>
@@ -10751,10 +10751,10 @@
         <v>15</v>
       </c>
       <c r="B27" s="1">
-        <v>220627</v>
+        <v>220829</v>
       </c>
       <c r="C27" s="1">
-        <v>0.67988</v>
+        <v>0.67926</v>
       </c>
       <c r="D27" s="1">
         <v>10000</v>
@@ -10793,10 +10793,10 @@
         <v>16</v>
       </c>
       <c r="B28" s="1">
-        <v>235156</v>
+        <v>235433</v>
       </c>
       <c r="C28" s="1">
-        <v>0.6804</v>
+        <v>0.6796</v>
       </c>
       <c r="D28" s="1">
         <v>10000</v>
@@ -10835,10 +10835,10 @@
         <v>31</v>
       </c>
       <c r="B29" s="1">
-        <v>387728</v>
+        <v>387616</v>
       </c>
       <c r="C29" s="1">
-        <v>0.79953</v>
+        <v>0.79976</v>
       </c>
       <c r="D29" s="1">
         <v>10000</v>
@@ -10877,10 +10877,10 @@
         <v>32</v>
       </c>
       <c r="B30" s="1">
-        <v>399975</v>
+        <v>400140</v>
       </c>
       <c r="C30" s="1">
-        <v>0.80005</v>
+        <v>0.79972</v>
       </c>
       <c r="D30" s="1">
         <v>10000</v>
@@ -10919,10 +10919,10 @@
         <v>63</v>
       </c>
       <c r="B31" s="1">
-        <v>521066</v>
+        <v>520790</v>
       </c>
       <c r="C31" s="1">
-        <v>1.20906</v>
+        <v>1.2097</v>
       </c>
       <c r="D31" s="1">
         <v>10000</v>
@@ -10961,10 +10961,10 @@
         <v>64</v>
       </c>
       <c r="B32" s="1">
-        <v>424175</v>
+        <v>423278</v>
       </c>
       <c r="C32" s="1">
-        <v>1.50881</v>
+        <v>1.51201</v>
       </c>
       <c r="D32" s="1">
         <v>10000</v>
@@ -11003,10 +11003,10 @@
         <v>127</v>
       </c>
       <c r="B33" s="1">
-        <v>653215</v>
+        <v>651817</v>
       </c>
       <c r="C33" s="1">
-        <v>1.94423</v>
+        <v>1.9484</v>
       </c>
       <c r="D33" s="1">
         <v>10000</v>
@@ -11045,10 +11045,10 @@
         <v>128</v>
       </c>
       <c r="B34" s="1">
-        <v>571988</v>
+        <v>571827</v>
       </c>
       <c r="C34" s="1">
-        <v>2.23781</v>
+        <v>2.23844</v>
       </c>
       <c r="D34" s="1">
         <v>10000</v>
@@ -11087,10 +11087,10 @@
         <v>255</v>
       </c>
       <c r="B35" s="1">
-        <v>752106</v>
+        <v>752250</v>
       </c>
       <c r="C35" s="1">
-        <v>3.39048</v>
+        <v>3.38983</v>
       </c>
       <c r="D35" s="1">
         <v>10000</v>
@@ -11129,10 +11129,10 @@
         <v>256</v>
       </c>
       <c r="B36" s="1">
-        <v>685115</v>
+        <v>682537</v>
       </c>
       <c r="C36" s="1">
-        <v>3.7366</v>
+        <v>3.75071</v>
       </c>
       <c r="D36" s="1">
         <v>10000</v>
@@ -11171,10 +11171,10 @@
         <v>511</v>
       </c>
       <c r="B37" s="1">
-        <v>791372</v>
+        <v>792150</v>
       </c>
       <c r="C37" s="1">
-        <v>6.45714</v>
+        <v>6.4508</v>
       </c>
       <c r="D37" s="1">
         <v>10000</v>
@@ -11213,10 +11213,10 @@
         <v>512</v>
       </c>
       <c r="B38" s="1">
-        <v>788199</v>
+        <v>787478</v>
       </c>
       <c r="C38" s="1">
-        <v>6.49582</v>
+        <v>6.50177</v>
       </c>
       <c r="D38" s="1">
         <v>10000</v>
@@ -11255,10 +11255,10 @@
         <v>1023</v>
       </c>
       <c r="B39" s="1">
-        <v>810372</v>
+        <v>810553</v>
       </c>
       <c r="C39" s="1">
-        <v>12.6238</v>
+        <v>12.621</v>
       </c>
       <c r="D39" s="1">
         <v>10000</v>
@@ -11297,10 +11297,10 @@
         <v>1024</v>
       </c>
       <c r="B40" s="1">
-        <v>813978</v>
+        <v>814001</v>
       </c>
       <c r="C40" s="1">
-        <v>12.5802</v>
+        <v>12.5798</v>
       </c>
       <c r="D40" s="1">
         <v>10000</v>
@@ -11339,10 +11339,10 @@
         <v>1</v>
       </c>
       <c r="B41" s="1">
-        <v>29157.1</v>
+        <v>29391</v>
       </c>
       <c r="C41" s="1">
-        <v>0.34297</v>
+        <v>0.34024</v>
       </c>
       <c r="D41" s="1">
         <v>10000</v>
@@ -11381,10 +11381,10 @@
         <v>2</v>
       </c>
       <c r="B42" s="1">
-        <v>57818.5</v>
+        <v>58056.8</v>
       </c>
       <c r="C42" s="1">
-        <v>0.34591</v>
+        <v>0.34449</v>
       </c>
       <c r="D42" s="1">
         <v>10000</v>
@@ -11423,10 +11423,10 @@
         <v>3</v>
       </c>
       <c r="B43" s="1">
-        <v>83280.1</v>
+        <v>82820.3</v>
       </c>
       <c r="C43" s="1">
-        <v>0.36023</v>
+        <v>0.36223</v>
       </c>
       <c r="D43" s="1">
         <v>10000</v>
@@ -11465,10 +11465,10 @@
         <v>4</v>
       </c>
       <c r="B44" s="1">
-        <v>109358</v>
+        <v>109233</v>
       </c>
       <c r="C44" s="1">
-        <v>0.36577</v>
+        <v>0.36619</v>
       </c>
       <c r="D44" s="1">
         <v>10000</v>
@@ -11507,10 +11507,10 @@
         <v>7</v>
       </c>
       <c r="B45" s="1">
-        <v>182734</v>
+        <v>181131</v>
       </c>
       <c r="C45" s="1">
-        <v>0.38307</v>
+        <v>0.38646</v>
       </c>
       <c r="D45" s="1">
         <v>10000</v>
@@ -11549,10 +11549,10 @@
         <v>8</v>
       </c>
       <c r="B46" s="1">
-        <v>207781</v>
+        <v>202650</v>
       </c>
       <c r="C46" s="1">
-        <v>0.38502</v>
+        <v>0.39477</v>
       </c>
       <c r="D46" s="1">
         <v>10000</v>
@@ -11591,10 +11591,10 @@
         <v>15</v>
       </c>
       <c r="B47" s="1">
-        <v>220653</v>
+        <v>219192</v>
       </c>
       <c r="C47" s="1">
-        <v>0.6798</v>
+        <v>0.68433</v>
       </c>
       <c r="D47" s="1">
         <v>10000</v>
@@ -11633,10 +11633,10 @@
         <v>16</v>
       </c>
       <c r="B48" s="1">
-        <v>235388</v>
+        <v>235135</v>
       </c>
       <c r="C48" s="1">
-        <v>0.67973</v>
+        <v>0.68046</v>
       </c>
       <c r="D48" s="1">
         <v>10000</v>
@@ -11675,10 +11675,10 @@
         <v>31</v>
       </c>
       <c r="B49" s="1">
-        <v>387932</v>
+        <v>387956</v>
       </c>
       <c r="C49" s="1">
-        <v>0.79911</v>
+        <v>0.79906</v>
       </c>
       <c r="D49" s="1">
         <v>10000</v>
@@ -11717,10 +11717,10 @@
         <v>32</v>
       </c>
       <c r="B50" s="1">
-        <v>400305</v>
+        <v>398159</v>
       </c>
       <c r="C50" s="1">
-        <v>0.79939</v>
+        <v>0.8037</v>
       </c>
       <c r="D50" s="1">
         <v>10000</v>
@@ -11759,10 +11759,10 @@
         <v>63</v>
       </c>
       <c r="B51" s="1">
-        <v>520571</v>
+        <v>520347</v>
       </c>
       <c r="C51" s="1">
-        <v>1.21021</v>
+        <v>1.21073</v>
       </c>
       <c r="D51" s="1">
         <v>10000</v>
@@ -11801,10 +11801,10 @@
         <v>64</v>
       </c>
       <c r="B52" s="1">
-        <v>423614</v>
+        <v>422942</v>
       </c>
       <c r="C52" s="1">
-        <v>1.51081</v>
+        <v>1.51321</v>
       </c>
       <c r="D52" s="1">
         <v>10000</v>
@@ -11843,10 +11843,10 @@
         <v>127</v>
       </c>
       <c r="B53" s="1">
-        <v>655690</v>
+        <v>652467</v>
       </c>
       <c r="C53" s="1">
-        <v>1.93689</v>
+        <v>1.94646</v>
       </c>
       <c r="D53" s="1">
         <v>10000</v>
@@ -11885,10 +11885,10 @@
         <v>128</v>
       </c>
       <c r="B54" s="1">
-        <v>572902</v>
+        <v>572134</v>
       </c>
       <c r="C54" s="1">
-        <v>2.23424</v>
+        <v>2.23724</v>
       </c>
       <c r="D54" s="1">
         <v>10000</v>
@@ -11927,10 +11927,10 @@
         <v>255</v>
       </c>
       <c r="B55" s="1">
-        <v>751855</v>
+        <v>752053</v>
       </c>
       <c r="C55" s="1">
-        <v>3.39161</v>
+        <v>3.39072</v>
       </c>
       <c r="D55" s="1">
         <v>10000</v>
@@ -11969,10 +11969,10 @@
         <v>256</v>
       </c>
       <c r="B56" s="1">
-        <v>685495</v>
+        <v>683768</v>
       </c>
       <c r="C56" s="1">
-        <v>3.73453</v>
+        <v>3.74396</v>
       </c>
       <c r="D56" s="1">
         <v>10000</v>
@@ -12011,10 +12011,10 @@
         <v>511</v>
       </c>
       <c r="B57" s="1">
-        <v>791237</v>
+        <v>792386</v>
       </c>
       <c r="C57" s="1">
-        <v>6.45824</v>
+        <v>6.44888</v>
       </c>
       <c r="D57" s="1">
         <v>10000</v>
@@ -12053,10 +12053,10 @@
         <v>512</v>
       </c>
       <c r="B58" s="1">
-        <v>787995</v>
+        <v>787645</v>
       </c>
       <c r="C58" s="1">
-        <v>6.4975</v>
+        <v>6.50039</v>
       </c>
       <c r="D58" s="1">
         <v>10000</v>
@@ -12095,10 +12095,10 @@
         <v>1023</v>
       </c>
       <c r="B59" s="1">
-        <v>809995</v>
+        <v>810844</v>
       </c>
       <c r="C59" s="1">
-        <v>12.6297</v>
+        <v>12.6165</v>
       </c>
       <c r="D59" s="1">
         <v>10000</v>
@@ -12137,10 +12137,10 @@
         <v>1024</v>
       </c>
       <c r="B60" s="1">
-        <v>813949</v>
+        <v>814052</v>
       </c>
       <c r="C60" s="1">
-        <v>12.5806</v>
+        <v>12.5791</v>
       </c>
       <c r="D60" s="1">
         <v>10000</v>
@@ -12179,10 +12179,10 @@
         <v>1</v>
       </c>
       <c r="B61" s="1">
-        <v>29368.6</v>
+        <v>29237.2</v>
       </c>
       <c r="C61" s="1">
-        <v>0.3405</v>
+        <v>0.34203</v>
       </c>
       <c r="D61" s="1">
         <v>10000</v>
@@ -12221,10 +12221,10 @@
         <v>2</v>
       </c>
       <c r="B62" s="1">
-        <v>58616.6</v>
+        <v>57865.3</v>
       </c>
       <c r="C62" s="1">
-        <v>0.3412</v>
+        <v>0.34563</v>
       </c>
       <c r="D62" s="1">
         <v>10000</v>
@@ -12263,10 +12263,10 @@
         <v>3</v>
       </c>
       <c r="B63" s="1">
-        <v>83224.7</v>
+        <v>83451.6</v>
       </c>
       <c r="C63" s="1">
-        <v>0.36047</v>
+        <v>0.35949</v>
       </c>
       <c r="D63" s="1">
         <v>10000</v>
@@ -12305,10 +12305,10 @@
         <v>4</v>
       </c>
       <c r="B64" s="1">
-        <v>109260</v>
+        <v>109391</v>
       </c>
       <c r="C64" s="1">
-        <v>0.3661</v>
+        <v>0.36566</v>
       </c>
       <c r="D64" s="1">
         <v>10000</v>
@@ -12347,10 +12347,10 @@
         <v>7</v>
       </c>
       <c r="B65" s="1">
-        <v>180231</v>
+        <v>175751</v>
       </c>
       <c r="C65" s="1">
-        <v>0.38839</v>
+        <v>0.39829</v>
       </c>
       <c r="D65" s="1">
         <v>10000</v>
@@ -12389,10 +12389,10 @@
         <v>8</v>
       </c>
       <c r="B66" s="1">
-        <v>208572</v>
+        <v>201147</v>
       </c>
       <c r="C66" s="1">
-        <v>0.38356</v>
+        <v>0.39772</v>
       </c>
       <c r="D66" s="1">
         <v>10000</v>
@@ -12431,10 +12431,10 @@
         <v>15</v>
       </c>
       <c r="B67" s="1">
-        <v>220287</v>
+        <v>220682</v>
       </c>
       <c r="C67" s="1">
-        <v>0.68093</v>
+        <v>0.67971</v>
       </c>
       <c r="D67" s="1">
         <v>10000</v>
@@ -12473,10 +12473,10 @@
         <v>16</v>
       </c>
       <c r="B68" s="1">
-        <v>235166</v>
+        <v>235353</v>
       </c>
       <c r="C68" s="1">
-        <v>0.68037</v>
+        <v>0.67983</v>
       </c>
       <c r="D68" s="1">
         <v>10000</v>
@@ -12515,10 +12515,10 @@
         <v>31</v>
       </c>
       <c r="B69" s="1">
-        <v>387563</v>
+        <v>387665</v>
       </c>
       <c r="C69" s="1">
-        <v>0.79987</v>
+        <v>0.79966</v>
       </c>
       <c r="D69" s="1">
         <v>10000</v>
@@ -12557,10 +12557,10 @@
         <v>32</v>
       </c>
       <c r="B70" s="1">
-        <v>400380</v>
+        <v>400110</v>
       </c>
       <c r="C70" s="1">
-        <v>0.79924</v>
+        <v>0.79978</v>
       </c>
       <c r="D70" s="1">
         <v>10000</v>
@@ -12599,10 +12599,10 @@
         <v>63</v>
       </c>
       <c r="B71" s="1">
-        <v>520635</v>
+        <v>520468</v>
       </c>
       <c r="C71" s="1">
-        <v>1.21006</v>
+        <v>1.21045</v>
       </c>
       <c r="D71" s="1">
         <v>10000</v>
@@ -12641,10 +12641,10 @@
         <v>64</v>
       </c>
       <c r="B72" s="1">
-        <v>422741</v>
+        <v>424533</v>
       </c>
       <c r="C72" s="1">
-        <v>1.51393</v>
+        <v>1.50754</v>
       </c>
       <c r="D72" s="1">
         <v>10000</v>
@@ -12683,10 +12683,10 @@
         <v>127</v>
       </c>
       <c r="B73" s="1">
-        <v>655173</v>
+        <v>653242</v>
       </c>
       <c r="C73" s="1">
-        <v>1.93842</v>
+        <v>1.94415</v>
       </c>
       <c r="D73" s="1">
         <v>10000</v>
@@ -12725,10 +12725,10 @@
         <v>128</v>
       </c>
       <c r="B74" s="1">
-        <v>573528</v>
+        <v>570901</v>
       </c>
       <c r="C74" s="1">
-        <v>2.2318</v>
+        <v>2.24207</v>
       </c>
       <c r="D74" s="1">
         <v>10000</v>
@@ -12767,10 +12767,10 @@
         <v>255</v>
       </c>
       <c r="B75" s="1">
-        <v>751955</v>
+        <v>752037</v>
       </c>
       <c r="C75" s="1">
-        <v>3.39116</v>
+        <v>3.39079</v>
       </c>
       <c r="D75" s="1">
         <v>10000</v>
@@ -12809,10 +12809,10 @@
         <v>256</v>
       </c>
       <c r="B76" s="1">
-        <v>684961</v>
+        <v>685384</v>
       </c>
       <c r="C76" s="1">
-        <v>3.73744</v>
+        <v>3.73513</v>
       </c>
       <c r="D76" s="1">
         <v>10000</v>
@@ -12851,10 +12851,10 @@
         <v>511</v>
       </c>
       <c r="B77" s="1">
-        <v>791606</v>
+        <v>792652</v>
       </c>
       <c r="C77" s="1">
-        <v>6.45523</v>
+        <v>6.44671</v>
       </c>
       <c r="D77" s="1">
         <v>10000</v>
@@ -12893,10 +12893,10 @@
         <v>512</v>
       </c>
       <c r="B78" s="1">
-        <v>788046</v>
+        <v>787654</v>
       </c>
       <c r="C78" s="1">
-        <v>6.49708</v>
+        <v>6.50032</v>
       </c>
       <c r="D78" s="1">
         <v>10000</v>
@@ -12935,10 +12935,10 @@
         <v>1023</v>
       </c>
       <c r="B79" s="1">
-        <v>809990</v>
+        <v>810703</v>
       </c>
       <c r="C79" s="1">
-        <v>12.6298</v>
+        <v>12.6187</v>
       </c>
       <c r="D79" s="1">
         <v>10000</v>
@@ -12977,10 +12977,10 @@
         <v>1024</v>
       </c>
       <c r="B80" s="1">
-        <v>813970</v>
+        <v>813942</v>
       </c>
       <c r="C80" s="1">
-        <v>12.5803</v>
+        <v>12.5808</v>
       </c>
       <c r="D80" s="1">
         <v>10000</v>
@@ -13019,10 +13019,10 @@
         <v>1</v>
       </c>
       <c r="B81" s="1">
-        <v>29419.6</v>
+        <v>29492.4</v>
       </c>
       <c r="C81" s="1">
-        <v>0.33991</v>
+        <v>0.33907</v>
       </c>
       <c r="D81" s="1">
         <v>10000</v>
@@ -13061,10 +13061,10 @@
         <v>2</v>
       </c>
       <c r="B82" s="1">
-        <v>58285.2</v>
+        <v>58344.8</v>
       </c>
       <c r="C82" s="1">
-        <v>0.34314</v>
+        <v>0.34279</v>
       </c>
       <c r="D82" s="1">
         <v>10000</v>
@@ -13103,10 +13103,10 @@
         <v>3</v>
       </c>
       <c r="B83" s="1">
-        <v>82955.4</v>
+        <v>83114</v>
       </c>
       <c r="C83" s="1">
-        <v>0.36164</v>
+        <v>0.36095</v>
       </c>
       <c r="D83" s="1">
         <v>10000</v>
@@ -13145,10 +13145,10 @@
         <v>4</v>
       </c>
       <c r="B84" s="1">
-        <v>109182</v>
+        <v>109215</v>
       </c>
       <c r="C84" s="1">
-        <v>0.36636</v>
+        <v>0.36625</v>
       </c>
       <c r="D84" s="1">
         <v>10000</v>
@@ -13187,10 +13187,10 @@
         <v>7</v>
       </c>
       <c r="B85" s="1">
-        <v>181507</v>
+        <v>182667</v>
       </c>
       <c r="C85" s="1">
-        <v>0.38566</v>
+        <v>0.38321</v>
       </c>
       <c r="D85" s="1">
         <v>10000</v>
@@ -13229,10 +13229,10 @@
         <v>8</v>
       </c>
       <c r="B86" s="1">
-        <v>201918</v>
+        <v>208529</v>
       </c>
       <c r="C86" s="1">
-        <v>0.3962</v>
+        <v>0.38364</v>
       </c>
       <c r="D86" s="1">
         <v>10000</v>
@@ -13271,10 +13271,10 @@
         <v>15</v>
       </c>
       <c r="B87" s="1">
-        <v>220216</v>
+        <v>219427</v>
       </c>
       <c r="C87" s="1">
-        <v>0.68115</v>
+        <v>0.6836</v>
       </c>
       <c r="D87" s="1">
         <v>10000</v>
@@ -13313,10 +13313,10 @@
         <v>16</v>
       </c>
       <c r="B88" s="1">
-        <v>235426</v>
+        <v>235211</v>
       </c>
       <c r="C88" s="1">
-        <v>0.67962</v>
+        <v>0.68024</v>
       </c>
       <c r="D88" s="1">
         <v>10000</v>
@@ -13345,10 +13345,10 @@
         <v>31</v>
       </c>
       <c r="B89" s="1">
-        <v>387355</v>
+        <v>387040</v>
       </c>
       <c r="C89" s="1">
-        <v>0.8003</v>
+        <v>0.80095</v>
       </c>
       <c r="D89" s="1">
         <v>10000</v>
@@ -13377,10 +13377,10 @@
         <v>32</v>
       </c>
       <c r="B90" s="1">
-        <v>400140</v>
+        <v>400155</v>
       </c>
       <c r="C90" s="1">
-        <v>0.79972</v>
+        <v>0.79969</v>
       </c>
       <c r="D90" s="1">
         <v>10000</v>
@@ -13409,10 +13409,10 @@
         <v>63</v>
       </c>
       <c r="B91" s="1">
-        <v>519305</v>
+        <v>521100</v>
       </c>
       <c r="C91" s="1">
-        <v>1.21316</v>
+        <v>1.20898</v>
       </c>
       <c r="D91" s="1">
         <v>10000</v>
@@ -13441,10 +13441,10 @@
         <v>64</v>
       </c>
       <c r="B92" s="1">
-        <v>424482</v>
+        <v>424420</v>
       </c>
       <c r="C92" s="1">
-        <v>1.50772</v>
+        <v>1.50794</v>
       </c>
       <c r="D92" s="1">
         <v>10000</v>
@@ -13473,10 +13473,10 @@
         <v>127</v>
       </c>
       <c r="B93" s="1">
-        <v>655105</v>
+        <v>652423</v>
       </c>
       <c r="C93" s="1">
-        <v>1.93862</v>
+        <v>1.94659</v>
       </c>
       <c r="D93" s="1">
         <v>10000</v>
@@ -13505,10 +13505,10 @@
         <v>128</v>
       </c>
       <c r="B94" s="1">
-        <v>573680</v>
+        <v>568970</v>
       </c>
       <c r="C94" s="1">
-        <v>2.23121</v>
+        <v>2.24968</v>
       </c>
       <c r="D94" s="1">
         <v>10000</v>
@@ -13537,10 +13537,10 @@
         <v>255</v>
       </c>
       <c r="B95" s="1">
-        <v>752055</v>
+        <v>751909</v>
       </c>
       <c r="C95" s="1">
-        <v>3.39071</v>
+        <v>3.39137</v>
       </c>
       <c r="D95" s="1">
         <v>10000</v>
@@ -13569,10 +13569,10 @@
         <v>256</v>
       </c>
       <c r="B96" s="1">
-        <v>685954</v>
+        <v>686022</v>
       </c>
       <c r="C96" s="1">
-        <v>3.73203</v>
+        <v>3.73166</v>
       </c>
       <c r="D96" s="1">
         <v>10000</v>
@@ -13601,10 +13601,10 @@
         <v>511</v>
       </c>
       <c r="B97" s="1">
-        <v>791703</v>
+        <v>792446</v>
       </c>
       <c r="C97" s="1">
-        <v>6.45444</v>
+        <v>6.44839</v>
       </c>
       <c r="D97" s="1">
         <v>10000</v>
@@ -13633,10 +13633,10 @@
         <v>512</v>
       </c>
       <c r="B98" s="1">
-        <v>787932</v>
+        <v>787841</v>
       </c>
       <c r="C98" s="1">
-        <v>6.49802</v>
+        <v>6.49877</v>
       </c>
       <c r="D98" s="1">
         <v>10000</v>
@@ -13665,10 +13665,10 @@
         <v>1023</v>
       </c>
       <c r="B99" s="1">
-        <v>810037</v>
+        <v>810804</v>
       </c>
       <c r="C99" s="1">
-        <v>12.6291</v>
+        <v>12.6171</v>
       </c>
       <c r="D99" s="1">
         <v>10000</v>
@@ -13697,10 +13697,10 @@
         <v>1024</v>
       </c>
       <c r="B100" s="1">
-        <v>813977</v>
+        <v>813926</v>
       </c>
       <c r="C100" s="1">
-        <v>12.5802</v>
+        <v>12.581</v>
       </c>
       <c r="D100" s="1">
         <v>10000</v>
@@ -13729,10 +13729,10 @@
         <v>1</v>
       </c>
       <c r="B101" s="1">
-        <v>29442.1</v>
+        <v>29348.8</v>
       </c>
       <c r="C101" s="1">
-        <v>0.33965</v>
+        <v>0.34073</v>
       </c>
       <c r="D101" s="1">
         <v>10000</v>
@@ -13761,10 +13761,10 @@
         <v>2</v>
       </c>
       <c r="B102" s="1">
-        <v>58046.7</v>
+        <v>59229.4</v>
       </c>
       <c r="C102" s="1">
-        <v>0.34455</v>
+        <v>0.33767</v>
       </c>
       <c r="D102" s="1">
         <v>10000</v>
@@ -13793,10 +13793,10 @@
         <v>3</v>
       </c>
       <c r="B103" s="1">
-        <v>82708.4</v>
+        <v>85130.5</v>
       </c>
       <c r="C103" s="1">
-        <v>0.36272</v>
+        <v>0.3524</v>
       </c>
       <c r="D103" s="1">
         <v>10000</v>
@@ -13825,10 +13825,10 @@
         <v>4</v>
       </c>
       <c r="B104" s="1">
-        <v>109236</v>
+        <v>109072</v>
       </c>
       <c r="C104" s="1">
-        <v>0.36618</v>
+        <v>0.36673</v>
       </c>
       <c r="D104" s="1">
         <v>10000</v>
@@ -13857,10 +13857,10 @@
         <v>7</v>
       </c>
       <c r="B105" s="1">
-        <v>176647</v>
+        <v>182254</v>
       </c>
       <c r="C105" s="1">
-        <v>0.39627</v>
+        <v>0.38408</v>
       </c>
       <c r="D105" s="1">
         <v>10000</v>
@@ -13889,10 +13889,10 @@
         <v>8</v>
       </c>
       <c r="B106" s="1">
-        <v>202122</v>
+        <v>208883</v>
       </c>
       <c r="C106" s="1">
-        <v>0.3958</v>
+        <v>0.38299</v>
       </c>
       <c r="D106" s="1">
         <v>10000</v>
@@ -13921,10 +13921,10 @@
         <v>15</v>
       </c>
       <c r="B107" s="1">
-        <v>219690</v>
+        <v>219684</v>
       </c>
       <c r="C107" s="1">
-        <v>0.68278</v>
+        <v>0.6828</v>
       </c>
       <c r="D107" s="1">
         <v>10000</v>
@@ -13953,10 +13953,10 @@
         <v>16</v>
       </c>
       <c r="B108" s="1">
-        <v>235294</v>
+        <v>235218</v>
       </c>
       <c r="C108" s="1">
-        <v>0.68</v>
+        <v>0.68022</v>
       </c>
       <c r="D108" s="1">
         <v>10000</v>
@@ -13985,10 +13985,10 @@
         <v>31</v>
       </c>
       <c r="B109" s="1">
-        <v>387820</v>
+        <v>387791</v>
       </c>
       <c r="C109" s="1">
-        <v>0.79934</v>
+        <v>0.7994</v>
       </c>
       <c r="D109" s="1">
         <v>10000</v>
@@ -14017,10 +14017,10 @@
         <v>32</v>
       </c>
       <c r="B110" s="1">
-        <v>400310</v>
+        <v>400325</v>
       </c>
       <c r="C110" s="1">
-        <v>0.79938</v>
+        <v>0.79935</v>
       </c>
       <c r="D110" s="1">
         <v>10000</v>
@@ -14049,10 +14049,10 @@
         <v>63</v>
       </c>
       <c r="B111" s="1">
-        <v>520339</v>
+        <v>520657</v>
       </c>
       <c r="C111" s="1">
-        <v>1.21075</v>
+        <v>1.21001</v>
       </c>
       <c r="D111" s="1">
         <v>10000</v>
@@ -14081,10 +14081,10 @@
         <v>64</v>
       </c>
       <c r="B112" s="1">
-        <v>424116</v>
+        <v>422010</v>
       </c>
       <c r="C112" s="1">
-        <v>1.50902</v>
+        <v>1.51655</v>
       </c>
       <c r="D112" s="1">
         <v>10000</v>
@@ -14113,10 +14113,10 @@
         <v>127</v>
       </c>
       <c r="B113" s="1">
-        <v>654541</v>
+        <v>650158</v>
       </c>
       <c r="C113" s="1">
-        <v>1.94029</v>
+        <v>1.95337</v>
       </c>
       <c r="D113" s="1">
         <v>10000</v>
@@ -14145,10 +14145,10 @@
         <v>128</v>
       </c>
       <c r="B114" s="1">
-        <v>572689</v>
+        <v>571834</v>
       </c>
       <c r="C114" s="1">
-        <v>2.23507</v>
+        <v>2.23841</v>
       </c>
       <c r="D114" s="1">
         <v>10000</v>
@@ -14177,10 +14177,10 @@
         <v>255</v>
       </c>
       <c r="B115" s="1">
-        <v>752057</v>
+        <v>752053</v>
       </c>
       <c r="C115" s="1">
-        <v>3.3907</v>
+        <v>3.39072</v>
       </c>
       <c r="D115" s="1">
         <v>10000</v>
@@ -14209,10 +14209,10 @@
         <v>256</v>
       </c>
       <c r="B116" s="1">
-        <v>685807</v>
+        <v>683936</v>
       </c>
       <c r="C116" s="1">
-        <v>3.73283</v>
+        <v>3.74304</v>
       </c>
       <c r="D116" s="1">
         <v>10000</v>
@@ -14241,10 +14241,10 @@
         <v>511</v>
       </c>
       <c r="B117" s="1">
-        <v>791682</v>
+        <v>792052</v>
       </c>
       <c r="C117" s="1">
-        <v>6.45461</v>
+        <v>6.4516</v>
       </c>
       <c r="D117" s="1">
         <v>10000</v>
@@ -14273,10 +14273,10 @@
         <v>512</v>
       </c>
       <c r="B118" s="1">
-        <v>787772</v>
+        <v>787735</v>
       </c>
       <c r="C118" s="1">
-        <v>6.49934</v>
+        <v>6.49965</v>
       </c>
       <c r="D118" s="1">
         <v>10000</v>
@@ -14305,10 +14305,10 @@
         <v>1023</v>
       </c>
       <c r="B119" s="1">
-        <v>810089</v>
+        <v>810762</v>
       </c>
       <c r="C119" s="1">
-        <v>12.6282</v>
+        <v>12.6178</v>
       </c>
       <c r="D119" s="1">
         <v>10000</v>
@@ -14337,10 +14337,10 @@
         <v>1024</v>
       </c>
       <c r="B120" s="1">
-        <v>814024</v>
+        <v>814100</v>
       </c>
       <c r="C120" s="1">
-        <v>12.5795</v>
+        <v>12.5783</v>
       </c>
       <c r="D120" s="1">
         <v>10000</v>
@@ -14369,10 +14369,10 @@
         <v>1</v>
       </c>
       <c r="B121" s="1">
-        <v>29242.3</v>
+        <v>29322.9</v>
       </c>
       <c r="C121" s="1">
-        <v>0.34197</v>
+        <v>0.34103</v>
       </c>
       <c r="D121" s="1">
         <v>10000</v>
@@ -14401,10 +14401,10 @@
         <v>2</v>
       </c>
       <c r="B122" s="1">
-        <v>58253</v>
+        <v>59192.6</v>
       </c>
       <c r="C122" s="1">
-        <v>0.34333</v>
+        <v>0.33788</v>
       </c>
       <c r="D122" s="1">
         <v>10000</v>
@@ -14433,10 +14433,10 @@
         <v>3</v>
       </c>
       <c r="B123" s="1">
-        <v>82710.7</v>
+        <v>82882.1</v>
       </c>
       <c r="C123" s="1">
-        <v>0.36271</v>
+        <v>0.36196</v>
       </c>
       <c r="D123" s="1">
         <v>10000</v>
@@ -14465,10 +14465,10 @@
         <v>4</v>
       </c>
       <c r="B124" s="1">
-        <v>109099</v>
+        <v>109230</v>
       </c>
       <c r="C124" s="1">
-        <v>0.36664</v>
+        <v>0.3662</v>
       </c>
       <c r="D124" s="1">
         <v>10000</v>
@@ -14497,10 +14497,10 @@
         <v>7</v>
       </c>
       <c r="B125" s="1">
-        <v>175840</v>
+        <v>181418</v>
       </c>
       <c r="C125" s="1">
-        <v>0.39809</v>
+        <v>0.38585</v>
       </c>
       <c r="D125" s="1">
         <v>10000</v>
@@ -14529,10 +14529,10 @@
         <v>8</v>
       </c>
       <c r="B126" s="1">
-        <v>202250</v>
+        <v>209046</v>
       </c>
       <c r="C126" s="1">
-        <v>0.39555</v>
+        <v>0.38269</v>
       </c>
       <c r="D126" s="1">
         <v>10000</v>
@@ -14561,10 +14561,10 @@
         <v>15</v>
       </c>
       <c r="B127" s="1">
-        <v>219729</v>
+        <v>220465</v>
       </c>
       <c r="C127" s="1">
-        <v>0.68266</v>
+        <v>0.68038</v>
       </c>
       <c r="D127" s="1">
         <v>10000</v>
@@ -14593,10 +14593,10 @@
         <v>16</v>
       </c>
       <c r="B128" s="1">
-        <v>235194</v>
+        <v>235156</v>
       </c>
       <c r="C128" s="1">
-        <v>0.68029</v>
+        <v>0.6804</v>
       </c>
       <c r="D128" s="1">
         <v>10000</v>
@@ -14625,10 +14625,10 @@
         <v>31</v>
       </c>
       <c r="B129" s="1">
-        <v>387757</v>
+        <v>387946</v>
       </c>
       <c r="C129" s="1">
-        <v>0.79947</v>
+        <v>0.79908</v>
       </c>
       <c r="D129" s="1">
         <v>10000</v>
@@ -14657,10 +14657,10 @@
         <v>32</v>
       </c>
       <c r="B130" s="1">
-        <v>400095</v>
+        <v>400360</v>
       </c>
       <c r="C130" s="1">
-        <v>0.79981</v>
+        <v>0.79928</v>
       </c>
       <c r="D130" s="1">
         <v>10000</v>
@@ -14689,10 +14689,10 @@
         <v>63</v>
       </c>
       <c r="B131" s="1">
-        <v>520433</v>
+        <v>520369</v>
       </c>
       <c r="C131" s="1">
-        <v>1.21053</v>
+        <v>1.21068</v>
       </c>
       <c r="D131" s="1">
         <v>10000</v>
@@ -14721,10 +14721,10 @@
         <v>64</v>
       </c>
       <c r="B132" s="1">
-        <v>424783</v>
+        <v>422880</v>
       </c>
       <c r="C132" s="1">
-        <v>1.50665</v>
+        <v>1.51343</v>
       </c>
       <c r="D132" s="1">
         <v>10000</v>
@@ -14753,10 +14753,10 @@
         <v>127</v>
       </c>
       <c r="B133" s="1">
-        <v>655497</v>
+        <v>653037</v>
       </c>
       <c r="C133" s="1">
-        <v>1.93746</v>
+        <v>1.94476</v>
       </c>
       <c r="D133" s="1">
         <v>10000</v>
@@ -14785,10 +14785,10 @@
         <v>128</v>
       </c>
       <c r="B134" s="1">
-        <v>572638</v>
+        <v>572469</v>
       </c>
       <c r="C134" s="1">
-        <v>2.23527</v>
+        <v>2.23593</v>
       </c>
       <c r="D134" s="1">
         <v>10000</v>
@@ -14817,10 +14817,10 @@
         <v>255</v>
       </c>
       <c r="B135" s="1">
-        <v>751858</v>
+        <v>752323</v>
       </c>
       <c r="C135" s="1">
-        <v>3.3916</v>
+        <v>3.3895</v>
       </c>
       <c r="D135" s="1">
         <v>10000</v>
@@ -14849,10 +14849,10 @@
         <v>256</v>
       </c>
       <c r="B136" s="1">
-        <v>686870</v>
+        <v>683764</v>
       </c>
       <c r="C136" s="1">
-        <v>3.72705</v>
+        <v>3.74398</v>
       </c>
       <c r="D136" s="1">
         <v>10000</v>
@@ -14881,10 +14881,10 @@
         <v>511</v>
       </c>
       <c r="B137" s="1">
-        <v>791123</v>
+        <v>791926</v>
       </c>
       <c r="C137" s="1">
-        <v>6.45917</v>
+        <v>6.45262</v>
       </c>
       <c r="D137" s="1">
         <v>10000</v>
@@ -14913,10 +14913,10 @@
         <v>512</v>
       </c>
       <c r="B138" s="1">
-        <v>787875</v>
+        <v>787801</v>
       </c>
       <c r="C138" s="1">
-        <v>6.49849</v>
+        <v>6.4991</v>
       </c>
       <c r="D138" s="1">
         <v>10000</v>
@@ -14945,10 +14945,10 @@
         <v>1023</v>
       </c>
       <c r="B139" s="1">
-        <v>809713</v>
+        <v>810298</v>
       </c>
       <c r="C139" s="1">
-        <v>12.6341</v>
+        <v>12.625</v>
       </c>
       <c r="D139" s="1">
         <v>10000</v>
@@ -14977,10 +14977,10 @@
         <v>1024</v>
       </c>
       <c r="B140" s="1">
-        <v>813954</v>
+        <v>813714</v>
       </c>
       <c r="C140" s="1">
-        <v>12.5806</v>
+        <v>12.5843</v>
       </c>
       <c r="D140" s="1">
         <v>10000</v>
@@ -15009,10 +15009,10 @@
         <v>1</v>
       </c>
       <c r="B141" s="1">
-        <v>29525.5</v>
+        <v>29497.7</v>
       </c>
       <c r="C141" s="1">
-        <v>0.33869</v>
+        <v>0.33901</v>
       </c>
       <c r="D141" s="1">
         <v>10000</v>
@@ -15041,10 +15041,10 @@
         <v>2</v>
       </c>
       <c r="B142" s="1">
-        <v>58131.1</v>
+        <v>58348.2</v>
       </c>
       <c r="C142" s="1">
-        <v>0.34405</v>
+        <v>0.34277</v>
       </c>
       <c r="D142" s="1">
         <v>10000</v>
@@ -15073,10 +15073,10 @@
         <v>3</v>
       </c>
       <c r="B143" s="1">
-        <v>82754.1</v>
+        <v>84779.3</v>
       </c>
       <c r="C143" s="1">
-        <v>0.36252</v>
+        <v>0.35386</v>
       </c>
       <c r="D143" s="1">
         <v>10000</v>
@@ -15105,10 +15105,10 @@
         <v>4</v>
       </c>
       <c r="B144" s="1">
-        <v>109105</v>
+        <v>109233</v>
       </c>
       <c r="C144" s="1">
-        <v>0.36662</v>
+        <v>0.36619</v>
       </c>
       <c r="D144" s="1">
         <v>10000</v>
@@ -15137,10 +15137,10 @@
         <v>7</v>
       </c>
       <c r="B145" s="1">
-        <v>182036</v>
+        <v>175986</v>
       </c>
       <c r="C145" s="1">
-        <v>0.38454</v>
+        <v>0.39776</v>
       </c>
       <c r="D145" s="1">
         <v>10000</v>
@@ -15169,10 +15169,10 @@
         <v>8</v>
       </c>
       <c r="B146" s="1">
-        <v>200557</v>
+        <v>201157</v>
       </c>
       <c r="C146" s="1">
-        <v>0.39889</v>
+        <v>0.3977</v>
       </c>
       <c r="D146" s="1">
         <v>10000</v>
@@ -15201,10 +15201,10 @@
         <v>15</v>
       </c>
       <c r="B147" s="1">
-        <v>219893</v>
+        <v>220900</v>
       </c>
       <c r="C147" s="1">
-        <v>0.68215</v>
+        <v>0.67904</v>
       </c>
       <c r="D147" s="1">
         <v>10000</v>
@@ -15233,10 +15233,10 @@
         <v>16</v>
       </c>
       <c r="B148" s="1">
-        <v>235090</v>
+        <v>235589</v>
       </c>
       <c r="C148" s="1">
-        <v>0.68059</v>
+        <v>0.67915</v>
       </c>
       <c r="D148" s="1">
         <v>10000</v>
@@ -15265,10 +15265,10 @@
         <v>31</v>
       </c>
       <c r="B149" s="1">
-        <v>387762</v>
+        <v>387534</v>
       </c>
       <c r="C149" s="1">
-        <v>0.79946</v>
+        <v>0.79993</v>
       </c>
       <c r="D149" s="1">
         <v>10000</v>
@@ -15297,10 +15297,10 @@
         <v>32</v>
       </c>
       <c r="B150" s="1">
-        <v>400410</v>
+        <v>400300</v>
       </c>
       <c r="C150" s="1">
-        <v>0.79918</v>
+        <v>0.7994</v>
       </c>
       <c r="D150" s="1">
         <v>10000</v>
@@ -15329,10 +15329,10 @@
         <v>63</v>
       </c>
       <c r="B151" s="1">
-        <v>518501</v>
+        <v>520588</v>
       </c>
       <c r="C151" s="1">
-        <v>1.21504</v>
+        <v>1.21017</v>
       </c>
       <c r="D151" s="1">
         <v>10000</v>
@@ -15361,10 +15361,10 @@
         <v>64</v>
       </c>
       <c r="B152" s="1">
-        <v>425068</v>
+        <v>423922</v>
       </c>
       <c r="C152" s="1">
-        <v>1.50564</v>
+        <v>1.50971</v>
       </c>
       <c r="D152" s="1">
         <v>10000</v>
@@ -15393,10 +15393,10 @@
         <v>127</v>
       </c>
       <c r="B153" s="1">
-        <v>655589</v>
+        <v>653400</v>
       </c>
       <c r="C153" s="1">
-        <v>1.93719</v>
+        <v>1.94368</v>
       </c>
       <c r="D153" s="1">
         <v>10000</v>
@@ -15425,10 +15425,10 @@
         <v>128</v>
       </c>
       <c r="B154" s="1">
-        <v>573189</v>
+        <v>571740</v>
       </c>
       <c r="C154" s="1">
-        <v>2.23312</v>
+        <v>2.23878</v>
       </c>
       <c r="D154" s="1">
         <v>10000</v>
@@ -15457,10 +15457,10 @@
         <v>255</v>
       </c>
       <c r="B155" s="1">
-        <v>751833</v>
+        <v>751689</v>
       </c>
       <c r="C155" s="1">
-        <v>3.39171</v>
+        <v>3.39236</v>
       </c>
       <c r="D155" s="1">
         <v>10000</v>
@@ -15489,10 +15489,10 @@
         <v>256</v>
       </c>
       <c r="B156" s="1">
-        <v>687738</v>
+        <v>684924</v>
       </c>
       <c r="C156" s="1">
-        <v>3.72235</v>
+        <v>3.73764</v>
       </c>
       <c r="D156" s="1">
         <v>10000</v>
@@ -15521,10 +15521,10 @@
         <v>511</v>
       </c>
       <c r="B157" s="1">
-        <v>791312</v>
+        <v>792330</v>
       </c>
       <c r="C157" s="1">
-        <v>6.45763</v>
+        <v>6.44933</v>
       </c>
       <c r="D157" s="1">
         <v>10000</v>
@@ -15553,10 +15553,10 @@
         <v>512</v>
       </c>
       <c r="B158" s="1">
-        <v>787804</v>
+        <v>787610</v>
       </c>
       <c r="C158" s="1">
-        <v>6.49908</v>
+        <v>6.50068</v>
       </c>
       <c r="D158" s="1">
         <v>10000</v>
@@ -15585,10 +15585,10 @@
         <v>1023</v>
       </c>
       <c r="B159" s="1">
-        <v>809952</v>
+        <v>810330</v>
       </c>
       <c r="C159" s="1">
-        <v>12.6304</v>
+        <v>12.6245</v>
       </c>
       <c r="D159" s="1">
         <v>10000</v>
@@ -15617,10 +15617,10 @@
         <v>1024</v>
       </c>
       <c r="B160" s="1">
-        <v>813950</v>
+        <v>814002</v>
       </c>
       <c r="C160" s="1">
-        <v>12.5806</v>
+        <v>12.5798</v>
       </c>
       <c r="D160" s="1">
         <v>10000</v>
@@ -15649,10 +15649,10 @@
         <v>1</v>
       </c>
       <c r="B161" s="1">
-        <v>29347.9</v>
+        <v>29716.8</v>
       </c>
       <c r="C161" s="1">
-        <v>0.34074</v>
+        <v>0.33651</v>
       </c>
       <c r="D161" s="1">
         <v>10000</v>
@@ -15681,10 +15681,10 @@
         <v>2</v>
       </c>
       <c r="B162" s="1">
-        <v>58038.3</v>
+        <v>58163.2</v>
       </c>
       <c r="C162" s="1">
-        <v>0.3446</v>
+        <v>0.34386</v>
       </c>
       <c r="D162" s="1">
         <v>10000</v>
@@ -15713,10 +15713,10 @@
         <v>3</v>
       </c>
       <c r="B163" s="1">
-        <v>83160.1</v>
+        <v>83402.8</v>
       </c>
       <c r="C163" s="1">
-        <v>0.36075</v>
+        <v>0.3597</v>
       </c>
       <c r="D163" s="1">
         <v>10000</v>
@@ -15745,10 +15745,10 @@
         <v>4</v>
       </c>
       <c r="B164" s="1">
-        <v>109299</v>
+        <v>109239</v>
       </c>
       <c r="C164" s="1">
-        <v>0.36597</v>
+        <v>0.36617</v>
       </c>
       <c r="D164" s="1">
         <v>10000</v>
@@ -15777,10 +15777,10 @@
         <v>7</v>
       </c>
       <c r="B165" s="1">
-        <v>181847</v>
+        <v>182610</v>
       </c>
       <c r="C165" s="1">
-        <v>0.38494</v>
+        <v>0.38333</v>
       </c>
       <c r="D165" s="1">
         <v>10000</v>
@@ -15809,10 +15809,10 @@
         <v>8</v>
       </c>
       <c r="B166" s="1">
-        <v>208057</v>
+        <v>201258</v>
       </c>
       <c r="C166" s="1">
-        <v>0.38451</v>
+        <v>0.3975</v>
       </c>
       <c r="D166" s="1">
         <v>10000</v>
@@ -15841,10 +15841,10 @@
         <v>15</v>
       </c>
       <c r="B167" s="1">
-        <v>220429</v>
+        <v>220501</v>
       </c>
       <c r="C167" s="1">
-        <v>0.68049</v>
+        <v>0.68027</v>
       </c>
       <c r="D167" s="1">
         <v>10000</v>
@@ -15873,10 +15873,10 @@
         <v>16</v>
       </c>
       <c r="B168" s="1">
-        <v>235384</v>
+        <v>234973</v>
       </c>
       <c r="C168" s="1">
-        <v>0.67974</v>
+        <v>0.68093</v>
       </c>
       <c r="D168" s="1">
         <v>10000</v>
@@ -15905,10 +15905,10 @@
         <v>31</v>
       </c>
       <c r="B169" s="1">
-        <v>387437</v>
+        <v>387888</v>
       </c>
       <c r="C169" s="1">
-        <v>0.80013</v>
+        <v>0.7992</v>
       </c>
       <c r="D169" s="1">
         <v>10000</v>
@@ -15937,10 +15937,10 @@
         <v>32</v>
       </c>
       <c r="B170" s="1">
-        <v>400125</v>
+        <v>400285</v>
       </c>
       <c r="C170" s="1">
-        <v>0.79975</v>
+        <v>0.79943</v>
       </c>
       <c r="D170" s="1">
         <v>10000</v>
@@ -15969,10 +15969,10 @@
         <v>63</v>
       </c>
       <c r="B171" s="1">
-        <v>520803</v>
+        <v>519438</v>
       </c>
       <c r="C171" s="1">
-        <v>1.20967</v>
+        <v>1.21285</v>
       </c>
       <c r="D171" s="1">
         <v>10000</v>
@@ -16001,10 +16001,10 @@
         <v>64</v>
       </c>
       <c r="B172" s="1">
-        <v>423844</v>
+        <v>424496</v>
       </c>
       <c r="C172" s="1">
-        <v>1.50999</v>
+        <v>1.50767</v>
       </c>
       <c r="D172" s="1">
         <v>10000</v>
@@ -16033,10 +16033,10 @@
         <v>127</v>
       </c>
       <c r="B173" s="1">
-        <v>655406</v>
+        <v>653158</v>
       </c>
       <c r="C173" s="1">
-        <v>1.93773</v>
+        <v>1.9444</v>
       </c>
       <c r="D173" s="1">
         <v>10000</v>
@@ -16065,10 +16065,10 @@
         <v>128</v>
       </c>
       <c r="B174" s="1">
-        <v>572563</v>
+        <v>571702</v>
       </c>
       <c r="C174" s="1">
-        <v>2.23556</v>
+        <v>2.23893</v>
       </c>
       <c r="D174" s="1">
         <v>10000</v>
@@ -16097,10 +16097,10 @@
         <v>255</v>
       </c>
       <c r="B175" s="1">
-        <v>751725</v>
+        <v>752081</v>
       </c>
       <c r="C175" s="1">
-        <v>3.3922</v>
+        <v>3.39059</v>
       </c>
       <c r="D175" s="1">
         <v>10000</v>
@@ -16129,10 +16129,10 @@
         <v>256</v>
       </c>
       <c r="B176" s="1">
-        <v>685899</v>
+        <v>684150</v>
       </c>
       <c r="C176" s="1">
-        <v>3.73233</v>
+        <v>3.74187</v>
       </c>
       <c r="D176" s="1">
         <v>10000</v>
@@ -16161,10 +16161,10 @@
         <v>511</v>
       </c>
       <c r="B177" s="1">
-        <v>791511</v>
+        <v>789936</v>
       </c>
       <c r="C177" s="1">
-        <v>6.45601</v>
+        <v>6.46888</v>
       </c>
       <c r="D177" s="1">
         <v>10000</v>
@@ -16193,10 +16193,10 @@
         <v>512</v>
       </c>
       <c r="B178" s="1">
-        <v>787644</v>
+        <v>787707</v>
       </c>
       <c r="C178" s="1">
-        <v>6.5004</v>
+        <v>6.49988</v>
       </c>
       <c r="D178" s="1">
         <v>10000</v>
@@ -16225,10 +16225,10 @@
         <v>1023</v>
       </c>
       <c r="B179" s="1">
-        <v>810452</v>
+        <v>810558</v>
       </c>
       <c r="C179" s="1">
-        <v>12.6226</v>
+        <v>12.6209</v>
       </c>
       <c r="D179" s="1">
         <v>10000</v>
@@ -16257,10 +16257,10 @@
         <v>1024</v>
       </c>
       <c r="B180" s="1">
-        <v>814018</v>
+        <v>814036</v>
       </c>
       <c r="C180" s="1">
-        <v>12.5796</v>
+        <v>12.5793</v>
       </c>
       <c r="D180" s="1">
         <v>10000</v>
@@ -16289,10 +16289,10 @@
         <v>1</v>
       </c>
       <c r="B181" s="1">
-        <v>29129</v>
+        <v>29679.8</v>
       </c>
       <c r="C181" s="1">
-        <v>0.3433</v>
+        <v>0.33693</v>
       </c>
       <c r="D181" s="1">
         <v>10000</v>
@@ -16321,10 +16321,10 @@
         <v>2</v>
       </c>
       <c r="B182" s="1">
-        <v>59319</v>
+        <v>59497.2</v>
       </c>
       <c r="C182" s="1">
-        <v>0.33716</v>
+        <v>0.33615</v>
       </c>
       <c r="D182" s="1">
         <v>10000</v>
@@ -16353,10 +16353,10 @@
         <v>3</v>
       </c>
       <c r="B183" s="1">
-        <v>83444.6</v>
+        <v>83282.4</v>
       </c>
       <c r="C183" s="1">
-        <v>0.35952</v>
+        <v>0.36022</v>
       </c>
       <c r="D183" s="1">
         <v>10000</v>
@@ -16385,10 +16385,10 @@
         <v>4</v>
       </c>
       <c r="B184" s="1">
-        <v>109254</v>
+        <v>109290</v>
       </c>
       <c r="C184" s="1">
-        <v>0.36612</v>
+        <v>0.366</v>
       </c>
       <c r="D184" s="1">
         <v>10000</v>
@@ -16417,10 +16417,10 @@
         <v>7</v>
       </c>
       <c r="B185" s="1">
-        <v>181993</v>
+        <v>182825</v>
       </c>
       <c r="C185" s="1">
-        <v>0.38463</v>
+        <v>0.38288</v>
       </c>
       <c r="D185" s="1">
         <v>10000</v>
@@ -16449,10 +16449,10 @@
         <v>8</v>
       </c>
       <c r="B186" s="1">
-        <v>208263</v>
+        <v>207781</v>
       </c>
       <c r="C186" s="1">
-        <v>0.38413</v>
+        <v>0.38502</v>
       </c>
       <c r="D186" s="1">
         <v>10000</v>
@@ -16481,10 +16481,10 @@
         <v>15</v>
       </c>
       <c r="B187" s="1">
-        <v>220287</v>
+        <v>219896</v>
       </c>
       <c r="C187" s="1">
-        <v>0.68093</v>
+        <v>0.68214</v>
       </c>
       <c r="D187" s="1">
         <v>10000</v>
@@ -16513,10 +16513,10 @@
         <v>16</v>
       </c>
       <c r="B188" s="1">
-        <v>235332</v>
+        <v>234980</v>
       </c>
       <c r="C188" s="1">
-        <v>0.67989</v>
+        <v>0.68091</v>
       </c>
       <c r="D188" s="1">
         <v>10000</v>
@@ -16545,10 +16545,10 @@
         <v>31</v>
       </c>
       <c r="B189" s="1">
-        <v>387825</v>
+        <v>387868</v>
       </c>
       <c r="C189" s="1">
-        <v>0.79933</v>
+        <v>0.79924</v>
       </c>
       <c r="D189" s="1">
         <v>10000</v>
@@ -16577,10 +16577,10 @@
         <v>32</v>
       </c>
       <c r="B190" s="1">
-        <v>400155</v>
+        <v>400150</v>
       </c>
       <c r="C190" s="1">
-        <v>0.79969</v>
+        <v>0.7997</v>
       </c>
       <c r="D190" s="1">
         <v>10000</v>
@@ -16609,10 +16609,10 @@
         <v>63</v>
       </c>
       <c r="B191" s="1">
-        <v>520696</v>
+        <v>520902</v>
       </c>
       <c r="C191" s="1">
-        <v>1.20992</v>
+        <v>1.20944</v>
       </c>
       <c r="D191" s="1">
         <v>10000</v>
@@ -16641,10 +16641,10 @@
         <v>64</v>
       </c>
       <c r="B192" s="1">
-        <v>425654</v>
+        <v>423160</v>
       </c>
       <c r="C192" s="1">
-        <v>1.50357</v>
+        <v>1.51243</v>
       </c>
       <c r="D192" s="1">
         <v>10000</v>
@@ -16673,10 +16673,10 @@
         <v>127</v>
       </c>
       <c r="B193" s="1">
-        <v>654670</v>
+        <v>651683</v>
       </c>
       <c r="C193" s="1">
-        <v>1.93991</v>
+        <v>1.9488</v>
       </c>
       <c r="D193" s="1">
         <v>10000</v>
@@ -16699,10 +16699,10 @@
         <v>128</v>
       </c>
       <c r="B194" s="1">
-        <v>571898</v>
+        <v>571720</v>
       </c>
       <c r="C194" s="1">
-        <v>2.23816</v>
+        <v>2.23886</v>
       </c>
       <c r="D194" s="1">
         <v>10000</v>
@@ -16725,10 +16725,10 @@
         <v>255</v>
       </c>
       <c r="B195" s="1">
-        <v>751957</v>
+        <v>752006</v>
       </c>
       <c r="C195" s="1">
-        <v>3.39115</v>
+        <v>3.39093</v>
       </c>
       <c r="D195" s="1">
         <v>10000</v>
@@ -16751,10 +16751,10 @@
         <v>256</v>
       </c>
       <c r="B196" s="1">
-        <v>685588</v>
+        <v>684446</v>
       </c>
       <c r="C196" s="1">
-        <v>3.73402</v>
+        <v>3.74025</v>
       </c>
       <c r="D196" s="1">
         <v>10000</v>
@@ -16777,10 +16777,10 @@
         <v>511</v>
       </c>
       <c r="B197" s="1">
-        <v>791739</v>
+        <v>792693</v>
       </c>
       <c r="C197" s="1">
-        <v>6.45415</v>
+        <v>6.44638</v>
       </c>
       <c r="D197" s="1">
         <v>10000</v>
@@ -16803,10 +16803,10 @@
         <v>512</v>
       </c>
       <c r="B198" s="1">
-        <v>788001</v>
+        <v>787465</v>
       </c>
       <c r="C198" s="1">
-        <v>6.49745</v>
+        <v>6.50188</v>
       </c>
       <c r="D198" s="1">
         <v>10000</v>
@@ -16829,10 +16829,10 @@
         <v>1023</v>
       </c>
       <c r="B199" s="1">
-        <v>810124</v>
+        <v>811092</v>
       </c>
       <c r="C199" s="1">
-        <v>12.6277</v>
+        <v>12.6126</v>
       </c>
       <c r="D199" s="1">
         <v>10000</v>
@@ -16855,10 +16855,10 @@
         <v>1024</v>
       </c>
       <c r="B200" s="1">
-        <v>814060</v>
+        <v>813806</v>
       </c>
       <c r="C200" s="1">
-        <v>12.5789</v>
+        <v>12.5829</v>
       </c>
       <c r="D200" s="1">
         <v>10000</v>

</xml_diff>